<commit_message>
Updated daily log and folder structure v3
</commit_message>
<xml_diff>
--- a/Project_documents/Daily_log_GA.xlsx
+++ b/Project_documents/Daily_log_GA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="780" windowWidth="20360" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -57,13 +57,22 @@
   </si>
   <si>
     <t xml:space="preserve">Writing on the project plan, lab </t>
+  </si>
+  <si>
+    <t>Getting started with UPPMAX, logging in and creating soft linkes. Learning how to find things in the directories.</t>
+  </si>
+  <si>
+    <t>Running my first analysis of the data using FastQC. Learning how to connect to a working node and running in interactive mode. Synchronizing everything with my git-repository. Creating gitignore-file to prevent adding to large files</t>
+  </si>
+  <si>
+    <t>Analyze result from fastQC and then do the DNA assembly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,7 +83,14 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,8 +105,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -117,11 +133,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -404,214 +420,222 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>43913</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>43914</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>43915</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>43916</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>43919</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>